<commit_message>
[doc]: Update journal de travail Sofiène CI/CD
</commit_message>
<xml_diff>
--- a/WIP/journaux de travaux/CI_CD_journalTravail_Belkhiria_Sofiene.xlsx
+++ b/WIP/journaux de travaux/CI_CD_journalTravail_Belkhiria_Sofiene.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\P_DevOps324-450\WIP\journaux de travaux\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F190D11-1F1A-4649-A589-D70EF1264E63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B37642-DC81-497B-A0F0-E9970C31118E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
   <si>
     <t>Auteur:</t>
   </si>
@@ -134,6 +134,24 @@
   </si>
   <si>
     <t>11.11.2024  au 10.01.2025</t>
+  </si>
+  <si>
+    <t>Planif projet</t>
+  </si>
+  <si>
+    <t>Création d'un container mongoDB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creation d'un container Backend se connectant a la db </t>
+  </si>
+  <si>
+    <t>Aide avec Mathis pour la mise en place du frontEnd</t>
+  </si>
+  <si>
+    <t>Création du github ainsi que du github Projects + création des journaux de travaux</t>
+  </si>
+  <si>
+    <t>M.Schaffter nous a présenter le projet</t>
   </si>
 </sst>
 </file>
@@ -1083,16 +1101,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1935,16 +1953,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.3235294117647059</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.52941176470588236</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.14705882352941177</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4130,7 +4148,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4185,7 +4203,7 @@
       <c r="B3" s="83"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>0 heures 0 minutes</v>
+        <v>2 heures 50 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4200,15 +4218,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="19">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>0</v>
+        <v>170</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4243,27 +4261,43 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="72" t="str">
+      <c r="A7" s="72">
         <f>IF(ISBLANK(B7),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B7))</f>
-        <v/>
-      </c>
-      <c r="B7" s="32"/>
+        <v>45</v>
+      </c>
+      <c r="B7" s="32">
+        <v>45602</v>
+      </c>
       <c r="C7" s="33"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="28"/>
+      <c r="D7" s="34">
+        <v>25</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>35</v>
+      </c>
       <c r="G7" s="44"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="73" t="str">
+      <c r="A8" s="73">
         <f>IF(ISBLANK(B8),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B8))</f>
-        <v/>
-      </c>
-      <c r="B8" s="36"/>
+        <v>45</v>
+      </c>
+      <c r="B8" s="36">
+        <v>45602</v>
+      </c>
       <c r="C8" s="37"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="28"/>
+      <c r="D8" s="38">
+        <v>30</v>
+      </c>
+      <c r="E8" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="28" t="s">
+        <v>36</v>
+      </c>
       <c r="G8" s="45"/>
       <c r="M8" t="s">
         <v>2</v>
@@ -4276,15 +4310,23 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="74" t="str">
+      <c r="A9" s="74">
         <f>IF(ISBLANK(B9),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B9))</f>
-        <v/>
-      </c>
-      <c r="B9" s="40"/>
+        <v>45</v>
+      </c>
+      <c r="B9" s="40">
+        <v>45602</v>
+      </c>
       <c r="C9" s="41"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="28"/>
+      <c r="D9" s="42">
+        <v>25</v>
+      </c>
+      <c r="E9" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>31</v>
+      </c>
       <c r="G9" s="46"/>
       <c r="M9" t="s">
         <v>19</v>
@@ -4297,15 +4339,23 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="73" t="str">
+      <c r="A10" s="73">
         <f>IF(ISBLANK(B10),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B10))</f>
-        <v/>
-      </c>
-      <c r="B10" s="36"/>
+        <v>45</v>
+      </c>
+      <c r="B10" s="36">
+        <v>45602</v>
+      </c>
       <c r="C10" s="37"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="28"/>
+      <c r="D10" s="38">
+        <v>20</v>
+      </c>
+      <c r="E10" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>32</v>
+      </c>
       <c r="G10" s="45"/>
       <c r="M10" t="s">
         <v>3</v>
@@ -4318,15 +4368,25 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="74" t="str">
+      <c r="A11" s="74">
         <f>IF(ISBLANK(B11),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B11))</f>
-        <v/>
-      </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="28"/>
+        <v>45</v>
+      </c>
+      <c r="B11" s="40">
+        <v>45602</v>
+      </c>
+      <c r="C11" s="41">
+        <v>1</v>
+      </c>
+      <c r="D11" s="42">
+        <v>5</v>
+      </c>
+      <c r="E11" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>33</v>
+      </c>
       <c r="G11" s="46"/>
       <c r="M11" t="s">
         <v>4</v>
@@ -4339,15 +4399,23 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="73" t="str">
+      <c r="A12" s="73">
         <f>IF(ISBLANK(B12),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B12))</f>
-        <v/>
-      </c>
-      <c r="B12" s="36"/>
+        <v>45</v>
+      </c>
+      <c r="B12" s="36">
+        <v>45602</v>
+      </c>
       <c r="C12" s="37"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="28"/>
+      <c r="D12" s="38">
+        <v>5</v>
+      </c>
+      <c r="E12" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>34</v>
+      </c>
       <c r="G12" s="45"/>
       <c r="N12">
         <v>5</v>
@@ -10766,11 +10834,11 @@
       </c>
       <c r="B6">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E6,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="C6">
         <f t="shared" ref="C6:C9" si="0">SUM(A6:B6)</f>
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="E6" s="21" t="str">
         <f>'Journal de travail'!M8</f>
@@ -10778,11 +10846,11 @@
       </c>
       <c r="F6" s="50" t="str">
         <f>QUOTIENT(SUM(A6:B6),60)&amp;" h "&amp;TEXT(MOD(SUM(A6:B6),60), "00")&amp;" min"</f>
-        <v>0 h 00 min</v>
-      </c>
-      <c r="G6" s="47" t="e">
+        <v>0 h 55 min</v>
+      </c>
+      <c r="G6" s="47">
         <f>SUM(A6:B6)/$C$10</f>
-        <v>#DIV/0!</v>
+        <v>0.3235294117647059</v>
       </c>
       <c r="L6" s="62" t="str">
         <f>'Journal de travail'!M8</f>
@@ -10799,15 +10867,15 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="E7" s="30" t="str">
         <f>'Journal de travail'!M9</f>
@@ -10815,11 +10883,11 @@
       </c>
       <c r="F7" s="55" t="str">
         <f t="shared" ref="F7:F10" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>0 h 00 min</v>
-      </c>
-      <c r="G7" s="56" t="e">
+        <v>1 h 30 min</v>
+      </c>
+      <c r="G7" s="56">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$10</f>
-        <v>#DIV/0!</v>
+        <v>0.52941176470588236</v>
       </c>
       <c r="L7" s="64" t="str">
         <f>'Journal de travail'!M9</f>
@@ -10854,9 +10922,9 @@
         <f t="shared" si="1"/>
         <v>0 h 00 min</v>
       </c>
-      <c r="G8" s="47" t="e">
+      <c r="G8" s="47">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="L8" s="65" t="str">
         <f>'Journal de travail'!M10</f>
@@ -10877,11 +10945,11 @@
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="E9" s="23" t="str">
         <f>'Journal de travail'!M11</f>
@@ -10889,11 +10957,11 @@
       </c>
       <c r="F9" s="55" t="str">
         <f t="shared" si="1"/>
-        <v>0 h 00 min</v>
-      </c>
-      <c r="G9" s="56" t="e">
+        <v>0 h 25 min</v>
+      </c>
+      <c r="G9" s="56">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0.14705882352941177</v>
       </c>
       <c r="L9" s="66" t="str">
         <f>'Journal de travail'!M11</f>
@@ -10910,26 +10978,26 @@
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>SUM(A6:A9)</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>0</v>
+        <v>170</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>0 h 00 min</v>
+        <v>2 h 50 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>0</v>
+        <v>3.2196969696969696E-2</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>
@@ -10973,26 +11041,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -11215,32 +11263,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11257,4 +11300,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[infra + journal travail] Mise en place du backend
</commit_message>
<xml_diff>
--- a/WIP/journaux de travaux/CI_CD_journalTravail_Belkhiria_Sofiene.xlsx
+++ b/WIP/journaux de travaux/CI_CD_journalTravail_Belkhiria_Sofiene.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\P_DevOps324-450\WIP\journaux de travaux\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B37642-DC81-497B-A0F0-E9970C31118E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F7D0018-270D-463C-9077-B9B54DDBAD34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
   <si>
     <t>Auteur:</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t>M.Schaffter nous a présenter le projet</t>
+  </si>
+  <si>
+    <t>Mise en place du container FrontEnd</t>
   </si>
 </sst>
 </file>
@@ -1104,7 +1107,7 @@
                   <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>90</c:v>
+                  <c:v>155</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1953,16 +1956,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.3235294117647059</c:v>
+                  <c:v>0.23404255319148937</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.52941176470588236</c:v>
+                  <c:v>0.65957446808510634</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.14705882352941177</c:v>
+                  <c:v>0.10638297872340426</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4203,7 +4206,7 @@
       <c r="B3" s="83"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>2 heures 50 minutes</v>
+        <v>3 heures 55 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4218,15 +4221,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="19">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>170</v>
+        <v>235</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4425,15 +4428,25 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="74" t="str">
+      <c r="A13" s="74">
         <f>IF(ISBLANK(B13),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B13))</f>
-        <v/>
-      </c>
-      <c r="B13" s="40"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="28"/>
+        <v>46</v>
+      </c>
+      <c r="B13" s="40">
+        <v>45609</v>
+      </c>
+      <c r="C13" s="41">
+        <v>1</v>
+      </c>
+      <c r="D13" s="42">
+        <v>5</v>
+      </c>
+      <c r="E13" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="28" t="s">
+        <v>37</v>
+      </c>
       <c r="G13" s="46"/>
       <c r="N13">
         <v>6</v>
@@ -10850,7 +10863,7 @@
       </c>
       <c r="G6" s="47">
         <f>SUM(A6:B6)/$C$10</f>
-        <v>0.3235294117647059</v>
+        <v>0.23404255319148937</v>
       </c>
       <c r="L6" s="62" t="str">
         <f>'Journal de travail'!M8</f>
@@ -10867,15 +10880,15 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>90</v>
+        <v>155</v>
       </c>
       <c r="E7" s="30" t="str">
         <f>'Journal de travail'!M9</f>
@@ -10883,11 +10896,11 @@
       </c>
       <c r="F7" s="55" t="str">
         <f t="shared" ref="F7:F10" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>1 h 30 min</v>
+        <v>2 h 35 min</v>
       </c>
       <c r="G7" s="56">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$10</f>
-        <v>0.52941176470588236</v>
+        <v>0.65957446808510634</v>
       </c>
       <c r="L7" s="64" t="str">
         <f>'Journal de travail'!M9</f>
@@ -10961,7 +10974,7 @@
       </c>
       <c r="G9" s="56">
         <f t="shared" si="2"/>
-        <v>0.14705882352941177</v>
+        <v>0.10638297872340426</v>
       </c>
       <c r="L9" s="66" t="str">
         <f>'Journal de travail'!M11</f>
@@ -10978,26 +10991,26 @@
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>SUM(A6:A9)</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>170</v>
+        <v>235</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>2 h 50 min</v>
+        <v>3 h 55 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>3.2196969696969696E-2</v>
+        <v>4.450757575757576E-2</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>
@@ -11041,6 +11054,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -11263,27 +11296,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11300,29 +11338,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[docs] Update journal de travail
</commit_message>
<xml_diff>
--- a/WIP/journaux de travaux/CI_CD_journalTravail_Belkhiria_Sofiene.xlsx
+++ b/WIP/journaux de travaux/CI_CD_journalTravail_Belkhiria_Sofiene.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\P_DevOps324-450\WIP\journaux de travaux\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F7D0018-270D-463C-9077-B9B54DDBAD34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C8FB638-52A7-4851-AC93-5F8BF78F2F8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
   <si>
     <t>Auteur:</t>
   </si>
@@ -155,6 +155,9 @@
   </si>
   <si>
     <t>Mise en place du container FrontEnd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stand up  meeting </t>
   </si>
 </sst>
 </file>
@@ -1104,7 +1107,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>55</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>155</c:v>
@@ -1956,16 +1959,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.23404255319148937</c:v>
+                  <c:v>0.28000000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.65957446808510634</c:v>
+                  <c:v>0.62</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.10638297872340426</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4206,7 +4209,7 @@
       <c r="B3" s="83"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>3 heures 55 minutes</v>
+        <v>4 heures 10 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4225,11 +4228,11 @@
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>115</v>
+        <v>130</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>235</v>
+        <v>250</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4456,15 +4459,23 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="73" t="str">
+      <c r="A14" s="73">
         <f>IF(ISBLANK(B14),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B14))</f>
-        <v/>
-      </c>
-      <c r="B14" s="36"/>
+        <v>47</v>
+      </c>
+      <c r="B14" s="36">
+        <v>45616</v>
+      </c>
       <c r="C14" s="37"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="28"/>
+      <c r="D14" s="38">
+        <v>15</v>
+      </c>
+      <c r="E14" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="28" t="s">
+        <v>38</v>
+      </c>
       <c r="G14" s="45"/>
       <c r="N14">
         <v>7</v>
@@ -10847,11 +10858,11 @@
       </c>
       <c r="B6">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E6,'Journal de travail'!$D$7:$D$532)</f>
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="C6">
         <f t="shared" ref="C6:C9" si="0">SUM(A6:B6)</f>
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="E6" s="21" t="str">
         <f>'Journal de travail'!M8</f>
@@ -10859,11 +10870,11 @@
       </c>
       <c r="F6" s="50" t="str">
         <f>QUOTIENT(SUM(A6:B6),60)&amp;" h "&amp;TEXT(MOD(SUM(A6:B6),60), "00")&amp;" min"</f>
-        <v>0 h 55 min</v>
+        <v>1 h 10 min</v>
       </c>
       <c r="G6" s="47">
         <f>SUM(A6:B6)/$C$10</f>
-        <v>0.23404255319148937</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="L6" s="62" t="str">
         <f>'Journal de travail'!M8</f>
@@ -10900,7 +10911,7 @@
       </c>
       <c r="G7" s="56">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$10</f>
-        <v>0.65957446808510634</v>
+        <v>0.62</v>
       </c>
       <c r="L7" s="64" t="str">
         <f>'Journal de travail'!M9</f>
@@ -10974,7 +10985,7 @@
       </c>
       <c r="G9" s="56">
         <f t="shared" si="2"/>
-        <v>0.10638297872340426</v>
+        <v>0.1</v>
       </c>
       <c r="L9" s="66" t="str">
         <f>'Journal de travail'!M11</f>
@@ -10995,22 +11006,22 @@
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>115</v>
+        <v>130</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>235</v>
+        <v>250</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>3 h 55 min</v>
+        <v>4 h 10 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>4.450757575757576E-2</v>
+        <v>4.7348484848484848E-2</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>
@@ -11054,26 +11065,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -11296,32 +11287,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11338,4 +11324,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[doc]: (journal de travail) Update journal de travail
</commit_message>
<xml_diff>
--- a/WIP/journaux de travaux/CI_CD_journalTravail_Belkhiria_Sofiene.xlsx
+++ b/WIP/journaux de travaux/CI_CD_journalTravail_Belkhiria_Sofiene.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\P_DevOps324-450\WIP\journaux de travaux\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C8FB638-52A7-4851-AC93-5F8BF78F2F8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE724FDF-E1A9-4EDA-A32E-D3B796288EFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
   <si>
     <t>Auteur:</t>
   </si>
@@ -158,6 +158,9 @@
   </si>
   <si>
     <t xml:space="preserve">Stand up  meeting </t>
+  </si>
+  <si>
+    <t>Mise en place de la communication entre le frontend et le backend de la todo app</t>
   </si>
 </sst>
 </file>
@@ -1110,7 +1113,7 @@
                   <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>155</c:v>
+                  <c:v>235</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1959,16 +1962,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.28000000000000003</c:v>
+                  <c:v>0.21212121212121213</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.62</c:v>
+                  <c:v>0.71212121212121215</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.1</c:v>
+                  <c:v>7.575757575757576E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4154,7 +4157,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4209,7 +4212,7 @@
       <c r="B3" s="83"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>4 heures 10 minutes</v>
+        <v>5 heures 30 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4224,15 +4227,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="19">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>250</v>
+        <v>330</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4485,15 +4488,25 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="74" t="str">
+      <c r="A15" s="74">
         <f>IF(ISBLANK(B15),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B15))</f>
-        <v/>
-      </c>
-      <c r="B15" s="40"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="28"/>
+        <v>47</v>
+      </c>
+      <c r="B15" s="40">
+        <v>45616</v>
+      </c>
+      <c r="C15" s="41">
+        <v>1</v>
+      </c>
+      <c r="D15" s="42">
+        <v>20</v>
+      </c>
+      <c r="E15" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="28" t="s">
+        <v>39</v>
+      </c>
       <c r="G15" s="46"/>
       <c r="N15">
         <v>8</v>
@@ -10874,7 +10887,7 @@
       </c>
       <c r="G6" s="47">
         <f>SUM(A6:B6)/$C$10</f>
-        <v>0.28000000000000003</v>
+        <v>0.21212121212121213</v>
       </c>
       <c r="L6" s="62" t="str">
         <f>'Journal de travail'!M8</f>
@@ -10891,15 +10904,15 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>155</v>
+        <v>235</v>
       </c>
       <c r="E7" s="30" t="str">
         <f>'Journal de travail'!M9</f>
@@ -10907,11 +10920,11 @@
       </c>
       <c r="F7" s="55" t="str">
         <f t="shared" ref="F7:F10" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>2 h 35 min</v>
+        <v>3 h 55 min</v>
       </c>
       <c r="G7" s="56">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$10</f>
-        <v>0.62</v>
+        <v>0.71212121212121215</v>
       </c>
       <c r="L7" s="64" t="str">
         <f>'Journal de travail'!M9</f>
@@ -10985,7 +10998,7 @@
       </c>
       <c r="G9" s="56">
         <f t="shared" si="2"/>
-        <v>0.1</v>
+        <v>7.575757575757576E-2</v>
       </c>
       <c r="L9" s="66" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11002,26 +11015,26 @@
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>SUM(A6:A9)</f>
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>250</v>
+        <v>330</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>4 h 10 min</v>
+        <v>5 h 30 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>4.7348484848484848E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>
@@ -11065,6 +11078,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -11287,27 +11320,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11324,29 +11362,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[doc] update journal de travail CI/CD
</commit_message>
<xml_diff>
--- a/WIP/journaux de travaux/CI_CD_journalTravail_Belkhiria_Sofiene.xlsx
+++ b/WIP/journaux de travaux/CI_CD_journalTravail_Belkhiria_Sofiene.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\P_DevOps324-450\WIP\journaux de travaux\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A12E97-BF02-4A8B-8C07-91D1F4D239E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC946AE8-40C7-4474-B0F2-BA5FE29102B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="43">
   <si>
     <t>Auteur:</t>
   </si>
@@ -167,6 +167,9 @@
   </si>
   <si>
     <t>Absence</t>
+  </si>
+  <si>
+    <t>Ecriture du point 2.1 de la doc</t>
   </si>
 </sst>
 </file>
@@ -604,80 +607,6 @@
   <dxfs count="17">
     <dxf>
       <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -851,6 +780,80 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCCC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1106,7 +1109,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>185</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>280</c:v>
@@ -1115,7 +1118,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1958,16 +1961,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.37755102040816324</c:v>
+                  <c:v>0.35087719298245612</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.5714285714285714</c:v>
+                  <c:v>0.49122807017543857</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.1020408163265307E-2</c:v>
+                  <c:v>0.15789473684210525</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3946,18 +3949,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}" name="Table1" displayName="Table1" ref="A6:G532" totalsRowShown="0" headerRowDxfId="16" tableBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}" name="Table1" displayName="Table1" ref="A6:G532" totalsRowShown="0" headerRowDxfId="8" tableBorderDxfId="7">
   <autoFilter ref="A6:G532" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{315BA4B4-9BD9-AB4E-8D40-FABFA0BB2AEA}" name="Semaine" dataDxfId="14">
+    <tableColumn id="1" xr3:uid="{315BA4B4-9BD9-AB4E-8D40-FABFA0BB2AEA}" name="Semaine" dataDxfId="6">
       <calculatedColumnFormula>IF(ISBLANK(B7),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{503C31E9-854D-BF42-85AC-8DFA1376C4D8}" name="Jour" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{B35A0B98-71A0-BA4F-BFAB-00A05EA1F23A}" name="h.      " dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{BE4D837D-FC99-BA48-A82F-B8C8E4CE5BF8}" name="min." dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{A2DCC539-6D2A-B04A-BF8E-6FACE6268D1F}" name="Type" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{4EA406B9-7EF7-D547-AF98-5AD11BE168E9}" name="Description" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{1735360B-2647-6D42-A0E3-3425EE302FFD}" name="Remarques/problèmes" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{503C31E9-854D-BF42-85AC-8DFA1376C4D8}" name="Jour" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{B35A0B98-71A0-BA4F-BFAB-00A05EA1F23A}" name="h.      " dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{BE4D837D-FC99-BA48-A82F-B8C8E4CE5BF8}" name="min." dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{A2DCC539-6D2A-B04A-BF8E-6FACE6268D1F}" name="Type" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{4EA406B9-7EF7-D547-AF98-5AD11BE168E9}" name="Description" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{1735360B-2647-6D42-A0E3-3425EE302FFD}" name="Remarques/problèmes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4153,7 +4156,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
+      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4208,7 +4211,7 @@
       <c r="B3" s="82"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>8 heures 10 minutes</v>
+        <v>9 heures 30 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4223,15 +4226,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="19">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>240</v>
+        <v>300</v>
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>490</v>
+        <v>570</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4560,30 +4563,48 @@
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="73" t="str">
+      <c r="A18" s="73">
         <f>IF(ISBLANK(B18),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B18))</f>
-        <v/>
-      </c>
-      <c r="B18" s="40"/>
+        <v>48</v>
+      </c>
+      <c r="B18" s="40">
+        <v>45623</v>
+      </c>
       <c r="C18" s="41"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="28"/>
+      <c r="D18" s="42">
+        <v>15</v>
+      </c>
+      <c r="E18" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" s="28" t="s">
+        <v>38</v>
+      </c>
       <c r="G18" s="45"/>
       <c r="O18">
         <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="74" t="str">
+      <c r="A19" s="74">
         <f>IF(ISBLANK(B19),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B19))</f>
-        <v/>
-      </c>
-      <c r="B19" s="36"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="28"/>
+        <v>48</v>
+      </c>
+      <c r="B19" s="36">
+        <v>45623</v>
+      </c>
+      <c r="C19" s="37">
+        <v>1</v>
+      </c>
+      <c r="D19" s="38">
+        <v>5</v>
+      </c>
+      <c r="E19" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="28" t="s">
+        <v>42</v>
+      </c>
       <c r="G19" s="46"/>
       <c r="O19">
         <v>55</v>
@@ -10754,28 +10775,28 @@
     <mergeCell ref="A3:B3"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:E532">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="16" priority="1">
       <formula>$E7="Autre"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="2" stopIfTrue="1">
       <formula>$E7="Design"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="3" stopIfTrue="1">
       <formula>$E7="Présentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="4" stopIfTrue="1">
       <formula>$E7="Meeting"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="5" stopIfTrue="1">
       <formula>$E7="Documentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="6" stopIfTrue="1">
       <formula>$E7="Test"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="7" stopIfTrue="1">
       <formula>$E7="Analyse"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
       <formula>$E7="Développement"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10885,11 +10906,11 @@
       </c>
       <c r="B6">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E6,'Journal de travail'!$D$7:$D$532)</f>
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="C6">
         <f t="shared" ref="C6:C9" si="0">SUM(A6:B6)</f>
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="E6" s="21" t="str">
         <f>'Journal de travail'!M8</f>
@@ -10897,11 +10918,11 @@
       </c>
       <c r="F6" s="50" t="str">
         <f>QUOTIENT(SUM(A6:B6),60)&amp;" h "&amp;TEXT(MOD(SUM(A6:B6),60), "00")&amp;" min"</f>
-        <v>3 h 05 min</v>
+        <v>3 h 20 min</v>
       </c>
       <c r="G6" s="47">
         <f>SUM(A6:B6)/$C$10</f>
-        <v>0.37755102040816324</v>
+        <v>0.35087719298245612</v>
       </c>
       <c r="L6" s="62" t="str">
         <f>'Journal de travail'!M8</f>
@@ -10938,7 +10959,7 @@
       </c>
       <c r="G7" s="56">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$10</f>
-        <v>0.5714285714285714</v>
+        <v>0.49122807017543857</v>
       </c>
       <c r="L7" s="64" t="str">
         <f>'Journal de travail'!M9</f>
@@ -10992,15 +11013,15 @@
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$D$7:$D$532)</f>
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>90</v>
       </c>
       <c r="E9" s="23" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11008,11 +11029,11 @@
       </c>
       <c r="F9" s="55" t="str">
         <f t="shared" si="1"/>
-        <v>0 h 25 min</v>
+        <v>1 h 30 min</v>
       </c>
       <c r="G9" s="56">
         <f t="shared" si="2"/>
-        <v>5.1020408163265307E-2</v>
+        <v>0.15789473684210525</v>
       </c>
       <c r="L9" s="66" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11029,26 +11050,26 @@
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>SUM(A6:A9)</f>
-        <v>240</v>
+        <v>300</v>
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>490</v>
+        <v>570</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>8 h 10 min</v>
+        <v>9 h 30 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>9.2803030303030304E-2</v>
+        <v>0.10795454545454546</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>
@@ -11092,6 +11113,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -11314,27 +11355,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11351,29 +11397,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[doc] (Rapport CI/CD) Updates des journaux de travaux CI/CD
</commit_message>
<xml_diff>
--- a/WIP/journaux de travaux/CI_CD_journalTravail_Belkhiria_Sofiene.xlsx
+++ b/WIP/journaux de travaux/CI_CD_journalTravail_Belkhiria_Sofiene.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\P_DevOps324-450\WIP\journaux de travaux\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC946AE8-40C7-4474-B0F2-BA5FE29102B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29CB258A-DFE8-4FC1-B8AC-246E9CBE42E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
   <si>
     <t>Auteur:</t>
   </si>
@@ -170,6 +170,9 @@
   </si>
   <si>
     <t>Ecriture du point 2.1 de la doc</t>
+  </si>
+  <si>
+    <t>Mise en place du workflow Test &amp; audit &amp; lint</t>
   </si>
 </sst>
 </file>
@@ -1112,7 +1115,7 @@
                   <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>280</c:v>
+                  <c:v>345</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1961,16 +1964,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.35087719298245612</c:v>
+                  <c:v>0.31496062992125984</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.49122807017543857</c:v>
+                  <c:v>0.54330708661417326</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.15789473684210525</c:v>
+                  <c:v>0.14173228346456693</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4156,7 +4159,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4211,7 +4214,7 @@
       <c r="B3" s="82"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>9 heures 30 minutes</v>
+        <v>10 heures 35 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4226,15 +4229,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="19">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>300</v>
+        <v>360</v>
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>570</v>
+        <v>635</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4611,15 +4614,25 @@
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="73" t="str">
+      <c r="A20" s="73">
         <f>IF(ISBLANK(B20),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B20))</f>
-        <v/>
-      </c>
-      <c r="B20" s="36"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="28"/>
+        <v>48</v>
+      </c>
+      <c r="B20" s="36">
+        <v>45623</v>
+      </c>
+      <c r="C20" s="37">
+        <v>1</v>
+      </c>
+      <c r="D20" s="38">
+        <v>5</v>
+      </c>
+      <c r="E20" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="28" t="s">
+        <v>43</v>
+      </c>
       <c r="G20" s="45"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -10922,7 +10935,7 @@
       </c>
       <c r="G6" s="47">
         <f>SUM(A6:B6)/$C$10</f>
-        <v>0.35087719298245612</v>
+        <v>0.31496062992125984</v>
       </c>
       <c r="L6" s="62" t="str">
         <f>'Journal de travail'!M8</f>
@@ -10939,15 +10952,15 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>180</v>
+        <v>240</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>280</v>
+        <v>345</v>
       </c>
       <c r="E7" s="30" t="str">
         <f>'Journal de travail'!M9</f>
@@ -10955,11 +10968,11 @@
       </c>
       <c r="F7" s="55" t="str">
         <f t="shared" ref="F7:F10" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>4 h 40 min</v>
+        <v>5 h 45 min</v>
       </c>
       <c r="G7" s="56">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$10</f>
-        <v>0.49122807017543857</v>
+        <v>0.54330708661417326</v>
       </c>
       <c r="L7" s="64" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11033,7 +11046,7 @@
       </c>
       <c r="G9" s="56">
         <f t="shared" si="2"/>
-        <v>0.15789473684210525</v>
+        <v>0.14173228346456693</v>
       </c>
       <c r="L9" s="66" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11050,26 +11063,26 @@
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>SUM(A6:A9)</f>
-        <v>300</v>
+        <v>360</v>
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>570</v>
+        <v>635</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>9 h 30 min</v>
+        <v>10 h 35 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>0.10795454545454546</v>
+        <v>0.12026515151515152</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>
@@ -11113,26 +11126,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -11355,32 +11348,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11397,4 +11385,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[doc] (journaux de travaux): Update des journaux de travaux
</commit_message>
<xml_diff>
--- a/WIP/journaux de travaux/CI_CD_journalTravail_Belkhiria_Sofiene.xlsx
+++ b/WIP/journaux de travaux/CI_CD_journalTravail_Belkhiria_Sofiene.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\belkh\Documents\GitHub\P_DevOps324-450\WIP\journaux de travaux\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\P_DevOps324-450\WIP\journaux de travaux\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D072551D-FBEF-4976-B991-95BBF191D6DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A2B4302-AF56-41E9-8BE6-4E3BF90772EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="46">
   <si>
     <t>Auteur:</t>
   </si>
@@ -176,6 +176,9 @@
   </si>
   <si>
     <t>Ecriture de la description du workflow &amp; Mis en place du diagramme de flux du workflow</t>
+  </si>
+  <si>
+    <t>Auto-Evaluation 80% avec le prof</t>
   </si>
 </sst>
 </file>
@@ -613,80 +616,6 @@
   <dxfs count="17">
     <dxf>
       <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -860,6 +789,80 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCCC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1115,7 +1118,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>200</c:v>
+                  <c:v>225</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>345</c:v>
@@ -1967,16 +1970,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.29411764705882354</c:v>
+                  <c:v>0.31914893617021278</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.50735294117647056</c:v>
+                  <c:v>0.48936170212765956</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.19852941176470587</c:v>
+                  <c:v>0.19148936170212766</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3955,18 +3958,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}" name="Table1" displayName="Table1" ref="A6:G532" totalsRowShown="0" headerRowDxfId="16" tableBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}" name="Table1" displayName="Table1" ref="A6:G532" totalsRowShown="0" headerRowDxfId="8" tableBorderDxfId="7">
   <autoFilter ref="A6:G532" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{315BA4B4-9BD9-AB4E-8D40-FABFA0BB2AEA}" name="Semaine" dataDxfId="14">
+    <tableColumn id="1" xr3:uid="{315BA4B4-9BD9-AB4E-8D40-FABFA0BB2AEA}" name="Semaine" dataDxfId="6">
       <calculatedColumnFormula>IF(ISBLANK(B7),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{503C31E9-854D-BF42-85AC-8DFA1376C4D8}" name="Jour" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{B35A0B98-71A0-BA4F-BFAB-00A05EA1F23A}" name="h.      " dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{BE4D837D-FC99-BA48-A82F-B8C8E4CE5BF8}" name="min." dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{A2DCC539-6D2A-B04A-BF8E-6FACE6268D1F}" name="Type" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{4EA406B9-7EF7-D547-AF98-5AD11BE168E9}" name="Description" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{1735360B-2647-6D42-A0E3-3425EE302FFD}" name="Remarques/problèmes" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{503C31E9-854D-BF42-85AC-8DFA1376C4D8}" name="Jour" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{B35A0B98-71A0-BA4F-BFAB-00A05EA1F23A}" name="h.      " dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{BE4D837D-FC99-BA48-A82F-B8C8E4CE5BF8}" name="min." dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{A2DCC539-6D2A-B04A-BF8E-6FACE6268D1F}" name="Type" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{4EA406B9-7EF7-D547-AF98-5AD11BE168E9}" name="Description" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{1735360B-2647-6D42-A0E3-3425EE302FFD}" name="Remarques/problèmes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4162,7 +4165,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
+      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4217,7 +4220,7 @@
       <c r="B3" s="82"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>11 heures 20 minutes</v>
+        <v>11 heures 45 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4236,11 +4239,11 @@
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>320</v>
+        <v>345</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>680</v>
+        <v>705</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4659,15 +4662,23 @@
       <c r="G21" s="46"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="73" t="str">
+      <c r="A22" s="73">
         <f>IF(ISBLANK(B22),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B22))</f>
-        <v/>
-      </c>
-      <c r="B22" s="36"/>
+        <v>50</v>
+      </c>
+      <c r="B22" s="36">
+        <v>45637</v>
+      </c>
       <c r="C22" s="37"/>
-      <c r="D22" s="38"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="28"/>
+      <c r="D22" s="38">
+        <v>25</v>
+      </c>
+      <c r="E22" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="F22" s="28" t="s">
+        <v>45</v>
+      </c>
       <c r="G22" s="45"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -10799,28 +10810,28 @@
     <mergeCell ref="A3:B3"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:E532">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="16" priority="1">
       <formula>$E7="Autre"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="2" stopIfTrue="1">
       <formula>$E7="Design"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="3" stopIfTrue="1">
       <formula>$E7="Présentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="4" stopIfTrue="1">
       <formula>$E7="Meeting"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="5" stopIfTrue="1">
       <formula>$E7="Documentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="6" stopIfTrue="1">
       <formula>$E7="Test"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="7" stopIfTrue="1">
       <formula>$E7="Analyse"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
       <formula>$E7="Développement"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10930,11 +10941,11 @@
       </c>
       <c r="B6">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E6,'Journal de travail'!$D$7:$D$532)</f>
-        <v>140</v>
+        <v>165</v>
       </c>
       <c r="C6">
         <f t="shared" ref="C6:C9" si="0">SUM(A6:B6)</f>
-        <v>200</v>
+        <v>225</v>
       </c>
       <c r="E6" s="21" t="str">
         <f>'Journal de travail'!M8</f>
@@ -10942,11 +10953,11 @@
       </c>
       <c r="F6" s="50" t="str">
         <f>QUOTIENT(SUM(A6:B6),60)&amp;" h "&amp;TEXT(MOD(SUM(A6:B6),60), "00")&amp;" min"</f>
-        <v>3 h 20 min</v>
+        <v>3 h 45 min</v>
       </c>
       <c r="G6" s="47">
         <f>SUM(A6:B6)/$C$10</f>
-        <v>0.29411764705882354</v>
+        <v>0.31914893617021278</v>
       </c>
       <c r="L6" s="62" t="str">
         <f>'Journal de travail'!M8</f>
@@ -10983,7 +10994,7 @@
       </c>
       <c r="G7" s="56">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$10</f>
-        <v>0.50735294117647056</v>
+        <v>0.48936170212765956</v>
       </c>
       <c r="L7" s="64" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11057,7 +11068,7 @@
       </c>
       <c r="G9" s="56">
         <f t="shared" si="2"/>
-        <v>0.19852941176470587</v>
+        <v>0.19148936170212766</v>
       </c>
       <c r="L9" s="66" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11078,22 +11089,22 @@
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>320</v>
+        <v>345</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>680</v>
+        <v>705</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>11 h 20 min</v>
+        <v>11 h 45 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>0.12878787878787878</v>
+        <v>0.13352272727272727</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>
@@ -11137,12 +11148,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11369,20 +11382,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -11407,18 +11427,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[doc](journal de travail) Update journal de travail
</commit_message>
<xml_diff>
--- a/WIP/journaux de travaux/CI_CD_journalTravail_Belkhiria_Sofiene.xlsx
+++ b/WIP/journaux de travaux/CI_CD_journalTravail_Belkhiria_Sofiene.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\P_DevOps324-450\WIP\journaux de travaux\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A2B4302-AF56-41E9-8BE6-4E3BF90772EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07060AAA-5D28-45B2-B92B-3DB3C201C559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="47">
   <si>
     <t>Auteur:</t>
   </si>
@@ -179,6 +179,9 @@
   </si>
   <si>
     <t>Auto-Evaluation 80% avec le prof</t>
+  </si>
+  <si>
+    <t>Ecriture de l'analyse initiale dans le rapport</t>
   </si>
 </sst>
 </file>
@@ -1127,7 +1130,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>135</c:v>
+                  <c:v>185</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1970,16 +1973,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.31914893617021278</c:v>
+                  <c:v>0.29801324503311261</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.48936170212765956</c:v>
+                  <c:v>0.45695364238410596</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.19148936170212766</c:v>
+                  <c:v>0.24503311258278146</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4165,7 +4168,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
+      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4220,7 +4223,7 @@
       <c r="B3" s="82"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>11 heures 45 minutes</v>
+        <v>12 heures 35 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4239,11 +4242,11 @@
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>345</v>
+        <v>395</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>705</v>
+        <v>755</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4682,15 +4685,23 @@
       <c r="G22" s="45"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="74" t="str">
+      <c r="A23" s="74">
         <f>IF(ISBLANK(B23),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B23))</f>
-        <v/>
-      </c>
-      <c r="B23" s="40"/>
+        <v>50</v>
+      </c>
+      <c r="B23" s="40">
+        <v>45637</v>
+      </c>
       <c r="C23" s="41"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="28"/>
+      <c r="D23" s="42">
+        <v>50</v>
+      </c>
+      <c r="E23" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" s="28" t="s">
+        <v>46</v>
+      </c>
       <c r="G23" s="46"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -10957,7 +10968,7 @@
       </c>
       <c r="G6" s="47">
         <f>SUM(A6:B6)/$C$10</f>
-        <v>0.31914893617021278</v>
+        <v>0.29801324503311261</v>
       </c>
       <c r="L6" s="62" t="str">
         <f>'Journal de travail'!M8</f>
@@ -10994,7 +11005,7 @@
       </c>
       <c r="G7" s="56">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$10</f>
-        <v>0.48936170212765956</v>
+        <v>0.45695364238410596</v>
       </c>
       <c r="L7" s="64" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11052,11 +11063,11 @@
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$D$7:$D$532)</f>
-        <v>75</v>
+        <v>125</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>135</v>
+        <v>185</v>
       </c>
       <c r="E9" s="23" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11064,11 +11075,11 @@
       </c>
       <c r="F9" s="55" t="str">
         <f t="shared" si="1"/>
-        <v>2 h 15 min</v>
+        <v>3 h 05 min</v>
       </c>
       <c r="G9" s="56">
         <f t="shared" si="2"/>
-        <v>0.19148936170212766</v>
+        <v>0.24503311258278146</v>
       </c>
       <c r="L9" s="66" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11089,22 +11100,22 @@
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>345</v>
+        <v>395</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>705</v>
+        <v>755</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>11 h 45 min</v>
+        <v>12 h 35 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>0.13352272727272727</v>
+        <v>0.14299242424242425</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>
@@ -11148,14 +11159,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11382,27 +11391,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -11427,9 +11429,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>